<commit_message>
Modifying results in table forms.
</commit_message>
<xml_diff>
--- a/svd/results.xlsx
+++ b/svd/results.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Correlations" sheetId="1" r:id="rId1"/>
+    <sheet name="Correlation 2 digits" sheetId="2" r:id="rId2"/>
+    <sheet name="Areas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
   <si>
     <t>Subject  1</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>0.5 External Sources</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V1/V1</t>
+  </si>
+  <si>
+    <t>V2/V1</t>
+  </si>
+  <si>
+    <t>V3/V1</t>
   </si>
 </sst>
 </file>
@@ -129,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +466,7 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -455,7 +477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -474,8 +496,17 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -497,8 +528,17 @@
       <c r="H3">
         <v>0.36399999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0.52</v>
+      </c>
+      <c r="K3">
+        <v>0.44</v>
+      </c>
+      <c r="L3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -520,8 +560,17 @@
       <c r="H4">
         <v>0.75180000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0.8327</v>
+      </c>
+      <c r="K4">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="L4">
+        <v>0.24310000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -543,8 +592,17 @@
       <c r="H5">
         <v>0.57569999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K5">
+        <v>0.85</v>
+      </c>
+      <c r="L5">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -566,8 +624,17 @@
       <c r="H6">
         <v>0.63219999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0.68759999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.4546</v>
+      </c>
+      <c r="L6">
+        <v>0.48370000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -589,8 +656,17 @@
       <c r="H7">
         <v>0.60199999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="K7">
+        <v>0.59760000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0.12970000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -612,8 +688,17 @@
       <c r="H8">
         <v>0.71830000000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0.43</v>
+      </c>
+      <c r="K8">
+        <v>0.73</v>
+      </c>
+      <c r="L8">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -635,8 +720,17 @@
       <c r="H9">
         <v>0.59699999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0.34</v>
+      </c>
+      <c r="K9">
+        <v>0.51</v>
+      </c>
+      <c r="L9">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -658,8 +752,17 @@
       <c r="H10">
         <v>0.49480000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0.88160000000000005</v>
+      </c>
+      <c r="K10">
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="L10">
+        <v>9.4399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -681,8 +784,17 @@
       <c r="H11">
         <v>0.71479999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0.77</v>
+      </c>
+      <c r="K11">
+        <v>0.37</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -704,8 +816,17 @@
       <c r="H12">
         <v>0.72009999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>0.92290000000000005</v>
+      </c>
+      <c r="K12">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="L12">
+        <v>0.42809999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -727,8 +848,17 @@
       <c r="H13">
         <v>0.49340000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0.67</v>
+      </c>
+      <c r="K13">
+        <v>0.51</v>
+      </c>
+      <c r="L13">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -750,8 +880,17 @@
       <c r="H14">
         <v>0.7601</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0.38</v>
+      </c>
+      <c r="K14">
+        <v>0.71</v>
+      </c>
+      <c r="L14">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -773,8 +912,17 @@
       <c r="H15">
         <v>0.47010000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>0.73</v>
+      </c>
+      <c r="K15">
+        <v>0.42</v>
+      </c>
+      <c r="L15">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -796,8 +944,17 @@
       <c r="H16">
         <v>0.64770000000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>0.66639999999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="L16">
+        <v>0.82479999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -819,8 +976,17 @@
       <c r="H17">
         <v>0.6925</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0.27260000000000001</v>
+      </c>
+      <c r="K17">
+        <v>0.47949999999999998</v>
+      </c>
+      <c r="L17">
+        <v>0.1095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -842,8 +1008,17 @@
       <c r="H18">
         <v>0.74970000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>0.85860000000000003</v>
+      </c>
+      <c r="K18">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="L18">
+        <v>0.2949</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -865,8 +1040,17 @@
       <c r="H19">
         <v>0.75390000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>0.85580000000000001</v>
+      </c>
+      <c r="K19">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="L19">
+        <v>0.32129999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -888,8 +1072,17 @@
       <c r="H20">
         <v>0.60580000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>0.21</v>
+      </c>
+      <c r="K20">
+        <v>0.01</v>
+      </c>
+      <c r="L20">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -911,8 +1104,17 @@
       <c r="H21">
         <v>0.67820000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>0.93769999999999998</v>
+      </c>
+      <c r="K21">
+        <v>0.71150000000000002</v>
+      </c>
+      <c r="L21">
+        <v>0.61860000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -933,6 +1135,56 @@
       </c>
       <c r="H22">
         <v>0.34520000000000001</v>
+      </c>
+      <c r="J22">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="K22">
+        <v>0.4889</v>
+      </c>
+      <c r="L22">
+        <v>0.27579999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <f>AVERAGE(B3:B22)</f>
+        <v>0.95810999999999991</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:L23" si="0">AVERAGE(C3:C22)</f>
+        <v>0.87926500000000019</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.6816350000000001</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.94977500000000004</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.85314499999999993</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.61836500000000016</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>0.63049500000000003</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0.54615499999999995</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>0.36769499999999999</v>
       </c>
     </row>
   </sheetData>
@@ -942,24 +1194,1395 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.99490000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.89490000000000003</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.79479999999999995</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.76890000000000003</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0.85760000000000003</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>0.8327</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.24310000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0.91320000000000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.57569999999999999</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.9909</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.65510000000000002</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.84060000000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.63219999999999998</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>0.68759999999999999</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.4546</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.48370000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.9698</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.81220000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.58560000000000001</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0.96120000000000005</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.86380000000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.59760000000000002</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.12970000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.9919</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.95930000000000004</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.84570000000000001</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.93569999999999998</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.71830000000000005</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>0.96209999999999996</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.95440000000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.63480000000000003</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0.97060000000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.7631</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.49480000000000002</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1">
+        <v>0.88160000000000005</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="L10" s="1">
+        <v>9.4399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.97350000000000003</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.88980000000000004</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.9274</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.73480000000000001</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.92630000000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.72009999999999996</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>0.92290000000000005</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.42809999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.9839</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.85860000000000003</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.82340000000000002</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.49340000000000001</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.99560000000000004</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.78049999999999997</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.7601</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.59960000000000002</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>0.75460000000000005</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.45610000000000001</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.47010000000000002</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.61309999999999998</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0.99529999999999996</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.64770000000000005</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
+        <v>0.66639999999999999</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.82479999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.9405</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.94940000000000002</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.6925</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1">
+        <v>0.27260000000000001</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.47949999999999998</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.1095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.78710000000000002</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.96860000000000002</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <v>0.85860000000000003</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.2949</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.95569999999999999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.87450000000000006</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.78210000000000002</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>0.95230000000000004</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.86180000000000001</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.75390000000000001</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <v>0.85580000000000001</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.32129999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.69869999999999999</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.873</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>0.9909</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.87570000000000003</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.67820000000000003</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1">
+        <v>0.93769999999999998</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.71150000000000002</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.61860000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.8488</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.65669999999999995</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.54320000000000002</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>0.8115</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.48039999999999999</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.4889</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.27579999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1">
+        <f>AVERAGE(B3:B22)</f>
+        <v>0.95810999999999991</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" ref="C23:L23" si="0">AVERAGE(C3:C22)</f>
+        <v>0.87926500000000019</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.6816350000000001</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.94977500000000004</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.85314499999999993</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61836500000000016</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63049500000000003</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54615499999999995</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.36769499999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.36</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.78</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <f>B2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <f>C2/B2</f>
+        <v>0.79194630872483218</v>
+      </c>
+      <c r="H2" s="1">
+        <f>D2/B2</f>
+        <v>0.59731543624161076</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.59</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.48</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F22" si="0">B3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G21" si="1">C3/B3</f>
+        <v>0.96935933147632314</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H22" si="2">D3/B3</f>
+        <v>0.69916434540389971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1702127659574468</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.82269503546099287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91103202846975084</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83629893238434161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.66</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.13</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.97368421052631571</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.80075187969924799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93117408906882582</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61943319838056676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.74</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95470383275261328</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.87804878048780488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.93</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.37</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80887372013651881</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.86348122866894184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81679389312977102</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.70229007633587781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.12</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.47</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.69339622641509424</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.59433962264150941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.44</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.85026737967914434</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.77005347593582885</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.79</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.96</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0949720670391061</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.94413407821229045</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.79</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.77</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.73</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.98882681564245811</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.96648044692737423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.31</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.87445887445887449</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.72727272727272718</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82198952879581155</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.70680628272251311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.92783505154639179</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.72680412371134018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93518518518518512</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.78240740740740733</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.86</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.74698795180722888</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.50200803212851397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.83</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84771573604060912</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.92893401015228427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.89805825242718451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1">
+        <f>AVERAGE(B2:B21)</f>
+        <v>2.4080000000000004</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" ref="C22:D22" si="3">AVERAGE(C2:C21)</f>
+        <v>2.1815000000000002</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8345000000000002</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.76183554817275745</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>